<commit_message>
All footprints now assigned
</commit_message>
<xml_diff>
--- a/keyboardFirmwareBuilder/switchFootprints.xlsx
+++ b/keyboardFirmwareBuilder/switchFootprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\a2000Serotina\a2000Serotina\keyboardFirmwareBuilder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71397EDF-DEB2-4F2F-BDFF-EA61D9A70504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9A0CFF-24BE-40D4-8FAC-6F2F2CEB790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5940" yWindow="1800" windowWidth="31455" windowHeight="17445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="213">
   <si>
     <t>Switch</t>
   </si>
@@ -154,14 +154,532 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>MX18</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>MX19</t>
+  </si>
+  <si>
+    <t>BSLS</t>
+  </si>
+  <si>
+    <t>MX20</t>
+  </si>
+  <si>
+    <t>DOT</t>
+  </si>
+  <si>
+    <t>MX21</t>
+  </si>
+  <si>
+    <t>LGUI</t>
+  </si>
+  <si>
+    <t>MX22</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>MX23</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>MX24</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>MX25</t>
+  </si>
+  <si>
+    <t>MX26</t>
+  </si>
+  <si>
+    <t>BSPC</t>
+  </si>
+  <si>
+    <t>MX-2U-NoLED</t>
+  </si>
+  <si>
+    <t>MX27</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>MX28</t>
+  </si>
+  <si>
+    <t>ENT</t>
+  </si>
+  <si>
+    <t>MX29</t>
+  </si>
+  <si>
+    <t>MX30</t>
+  </si>
+  <si>
+    <t>SCLN</t>
+  </si>
+  <si>
+    <t>MX31</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>MX32</t>
+  </si>
+  <si>
+    <t>SLSH</t>
+  </si>
+  <si>
+    <t>MX33</t>
+  </si>
+  <si>
+    <t>LALT</t>
+  </si>
+  <si>
+    <t>MX34</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>MX35</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>MX36</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>MX37</t>
+  </si>
+  <si>
+    <t>MX38</t>
+  </si>
+  <si>
+    <t>INS</t>
+  </si>
+  <si>
+    <t>MX39</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>MX40</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>MX41</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>MX42</t>
+  </si>
+  <si>
+    <t>QUOT</t>
+  </si>
+  <si>
+    <t>MX43</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>MX44</t>
+  </si>
+  <si>
+    <t>RSHIFT</t>
+  </si>
+  <si>
+    <t>MX-2.75U-NoLED</t>
+  </si>
+  <si>
+    <t>MX45</t>
+  </si>
+  <si>
+    <t>SPC</t>
+  </si>
+  <si>
+    <t>MX46</t>
+  </si>
+  <si>
+    <t>RGHT</t>
+  </si>
+  <si>
+    <t>MX-6.25U-NoLED</t>
+  </si>
+  <si>
+    <t>MX47</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>MX48</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>MX49</t>
+  </si>
+  <si>
+    <t>MX50</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>MX51</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>MX52</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>MX53</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>MX54</t>
+  </si>
+  <si>
+    <t>NUHS</t>
+  </si>
+  <si>
+    <t>MX55</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>MX56</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>MX57</t>
+  </si>
+  <si>
+    <t>RALT</t>
+  </si>
+  <si>
+    <t>MX58</t>
+  </si>
+  <si>
+    <t>MX59</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>MX60</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>MX61</t>
+  </si>
+  <si>
+    <t>MX63</t>
+  </si>
+  <si>
+    <t>MX62</t>
+  </si>
+  <si>
+    <t>PGUP</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>MX64</t>
+  </si>
+  <si>
+    <t>PGDN</t>
+  </si>
+  <si>
+    <t>MX65</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>MX66</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>MX67</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>MX68</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>MX69</t>
+  </si>
+  <si>
+    <t>RGUI</t>
+  </si>
+  <si>
+    <t>MX70</t>
+  </si>
+  <si>
+    <t>PDOT</t>
+  </si>
+  <si>
+    <t>MX71</t>
+  </si>
+  <si>
+    <t>MX72</t>
+  </si>
+  <si>
+    <t>NLCK</t>
+  </si>
+  <si>
+    <t>MX73</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>MX74</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>MX75</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>MX76</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>MX77</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>MX78</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>MX79</t>
+  </si>
+  <si>
+    <t>MENU</t>
+  </si>
+  <si>
+    <t>MX80</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>MX81</t>
+  </si>
+  <si>
+    <t>PSCR</t>
+  </si>
+  <si>
+    <t>MX82</t>
+  </si>
+  <si>
+    <t>MX83</t>
+  </si>
+  <si>
+    <t>PSLS</t>
+  </si>
+  <si>
+    <t>MX84</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>MX85</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>MX86</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>MX87</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>MX88</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>MX89</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>MX90</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>MX91</t>
+  </si>
+  <si>
+    <t>MX92</t>
+  </si>
+  <si>
+    <t>SLCK</t>
+  </si>
+  <si>
+    <t>MX93</t>
+  </si>
+  <si>
+    <t>PAST</t>
+  </si>
+  <si>
+    <t>MX94</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>MX95</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>MX96</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>MX97</t>
+  </si>
+  <si>
+    <t>PENT</t>
+  </si>
+  <si>
+    <t>MX98</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>MX99</t>
+  </si>
+  <si>
+    <t>PAUS</t>
+  </si>
+  <si>
+    <t>MX100</t>
+  </si>
+  <si>
+    <t>MX101</t>
+  </si>
+  <si>
+    <t>PMNS</t>
+  </si>
+  <si>
+    <t>MX102</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>MX103</t>
+  </si>
+  <si>
+    <t>PPLS</t>
+  </si>
+  <si>
+    <t>MX104</t>
+  </si>
+  <si>
+    <t>MX105</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -189,10 +707,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,20 +1008,20 @@
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -789,6 +1311,1502 @@
         <v>42</v>
       </c>
       <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>11</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>9</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>130</v>
+      </c>
+      <c r="B64">
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>9</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>11</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74">
+        <v>6</v>
+      </c>
+      <c r="C74">
+        <v>4</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75">
+        <v>6</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76">
+        <v>6</v>
+      </c>
+      <c r="C76">
+        <v>6</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>157</v>
+      </c>
+      <c r="B77">
+        <v>6</v>
+      </c>
+      <c r="C77">
+        <v>7</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>159</v>
+      </c>
+      <c r="B78">
+        <v>6</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>161</v>
+      </c>
+      <c r="B79">
+        <v>6</v>
+      </c>
+      <c r="C79">
+        <v>9</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82">
+        <v>7</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83" s="1">
+        <v>7</v>
+      </c>
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84">
+        <v>7</v>
+      </c>
+      <c r="C84">
+        <v>3</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85">
+        <v>7</v>
+      </c>
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>174</v>
+      </c>
+      <c r="B86">
+        <v>7</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>176</v>
+      </c>
+      <c r="B87">
+        <v>7</v>
+      </c>
+      <c r="C87">
+        <v>6</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+      <c r="C88">
+        <v>7</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89">
+        <v>7</v>
+      </c>
+      <c r="C89">
+        <v>8</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>182</v>
+      </c>
+      <c r="B90">
+        <v>7</v>
+      </c>
+      <c r="C90">
+        <v>9</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>184</v>
+      </c>
+      <c r="B91">
+        <v>8</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>186</v>
+      </c>
+      <c r="B92">
+        <v>8</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95">
+        <v>8</v>
+      </c>
+      <c r="C95">
+        <v>4</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>193</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>195</v>
+      </c>
+      <c r="B97">
+        <v>8</v>
+      </c>
+      <c r="C97">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>197</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+      <c r="C98">
+        <v>9</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E98" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>199</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>201</v>
+      </c>
+      <c r="B100">
+        <v>9</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>203</v>
+      </c>
+      <c r="B101">
+        <v>9</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1">
+        <v>9</v>
+      </c>
+      <c r="E101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102">
+        <v>9</v>
+      </c>
+      <c r="C102">
+        <v>3</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>206</v>
+      </c>
+      <c r="B103">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>208</v>
+      </c>
+      <c r="B104">
+        <v>9</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E104" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>211</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E106" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>